<commit_message>
Included agency data: - tree management - harvests etc
Updated cost calculations
</commit_message>
<xml_diff>
--- a/Data/data_agency.xlsx
+++ b/Data/data_agency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AA735B-6168-492A-86D3-61448638415E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC6FF53-9794-4B01-8A11-150E8D4CC14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="28695" yWindow="-8460" windowWidth="14610" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
   <si>
     <t>variable</t>
   </si>
@@ -71,9 +71,15 @@
     <t>percent/100</t>
   </si>
   <si>
+    <t>EUR/t</t>
+  </si>
+  <si>
     <t>Eur</t>
   </si>
   <si>
+    <t>h</t>
+  </si>
+  <si>
     <t>labor_wage_Eur_per_h_brutto</t>
   </si>
   <si>
@@ -92,12 +98,57 @@
     <t>walnut_price_wholesale_Eur_per_kg</t>
   </si>
   <si>
+    <t>fruit_time_to_first_yield_est</t>
+  </si>
+  <si>
+    <t>fruit_time_to_second_yield_est</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>timber_labor_harvest_mean_h</t>
+  </si>
+  <si>
     <t>fruit_price_machinery_mean_Eur</t>
   </si>
   <si>
     <t>fruit_price_machinery_var_Eur</t>
   </si>
   <si>
+    <t>Eur/ha</t>
+  </si>
+  <si>
+    <t>Einkommensstütze (GAP-Direktzahleung 1. Säule)</t>
+  </si>
+  <si>
+    <t>Eur/tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eur/tree </t>
+  </si>
+  <si>
+    <t>HALM 2.1 (Pflege von Agroforst, . Säule ökoregelung)</t>
+  </si>
+  <si>
+    <t>HALM 2.2 (Neupflanzung/Baum, Pflanzjahr)</t>
+  </si>
+  <si>
+    <t>HALM 2.2 (Neupflanzung/Baum, Folgejahre bis 5. Jahr)</t>
+  </si>
+  <si>
+    <t>tree_subsidies_HALM_2_1_annual_Eur_per_tree</t>
+  </si>
+  <si>
+    <t>tree_subsidies_HALM_2_2_y1_Eur_per_tree</t>
+  </si>
+  <si>
+    <t>tree_subsidies_HALM_2_2_y2_5_Eur_per_tree</t>
+  </si>
+  <si>
+    <t>tree_subsidies_GLOEZ_annual_Eur_per_ha</t>
+  </si>
+  <si>
     <t>absolute</t>
   </si>
   <si>
@@ -125,12 +176,6 @@
     <t>Variance in 1rst tree planting</t>
   </si>
   <si>
-    <t>fruit_labor_establishment_mean_h_per_tree</t>
-  </si>
-  <si>
-    <t>fruit_labor_establishment_var_per_tree</t>
-  </si>
-  <si>
     <t>tree_mainteance_costs_certificate</t>
   </si>
   <si>
@@ -156,6 +201,111 @@
   </si>
   <si>
     <t>Variance in machinery  (20 %, own estimate)</t>
+  </si>
+  <si>
+    <t>labor_fruit_pruning_juvenile_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_management_juvenile_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_pruning_expanding_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_management_expanding_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_harvest_expanding_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_harvest_mature_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_management_mature_h</t>
+  </si>
+  <si>
+    <t>labor_fruit_pruning_mature_h</t>
+  </si>
+  <si>
+    <t>Labor of annual shape pruning for juvenile trees (Report: 0.2)</t>
+  </si>
+  <si>
+    <t>Labor of annual shape pruning for trees in expanding yields (Report: 0.2)</t>
+  </si>
+  <si>
+    <t>Labor of annual shape pruning for mature trees (Report: 0.1, every 3-4 years)</t>
+  </si>
+  <si>
+    <t>Labor of annual tree management (check for dieseases, weed removal, etc) - Report: 0.8</t>
+  </si>
+  <si>
+    <t>Labor of annual tree management (check for dieseases, weed removal, etc) - Report: 0.2</t>
+  </si>
+  <si>
+    <t>Labor of tree shaking and collecting nuts (Report: 0.2)</t>
+  </si>
+  <si>
+    <t>tree_labor_establishment_mean_h_per_tree</t>
+  </si>
+  <si>
+    <t>tree_labor_establishment_var_per_tree</t>
+  </si>
+  <si>
+    <t>labor_fruit_replanting_mean_h_per_tree</t>
+  </si>
+  <si>
+    <t>labor_fruit_replanting_var_per_tree</t>
+  </si>
+  <si>
+    <t>First yield after planting (Report: after 5 years)</t>
+  </si>
+  <si>
+    <t>Start of expading yield phase (Report: 12 Years)</t>
+  </si>
+  <si>
+    <t>Amount of wood to sell per tree (Report: 1.3 m^3</t>
+  </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>Price for timber per m3 (Report: 30 €)</t>
+  </si>
+  <si>
+    <t>Labor to harvest a tree (Report: 0.5 h)</t>
+  </si>
+  <si>
+    <t>timespan</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Simulation duration (one lifespan of a economically used walnut tree)</t>
+  </si>
+  <si>
+    <t>field_size_ha</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>Field size of study case</t>
+  </si>
+  <si>
+    <t>n_trees</t>
+  </si>
+  <si>
+    <t>Number of walnut trees intendet to plant</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>timber_yield_mean_m3_per_tree</t>
+  </si>
+  <si>
+    <t>timber_price_mean_Eur_m3</t>
   </si>
 </sst>
 </file>
@@ -602,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,27 +788,27 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>1.05</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>1.05</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>9</v>
@@ -673,15 +823,15 @@
         <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -696,18 +846,18 @@
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -722,12 +872,12 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
@@ -742,15 +892,15 @@
         <v>100</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>9</v>
@@ -765,15 +915,15 @@
         <v>0.72</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
@@ -788,18 +938,18 @@
         <v>0.2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>1000</v>
@@ -811,15 +961,15 @@
         <v>1000</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>9</v>
@@ -834,15 +984,15 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>7</v>
@@ -857,18 +1007,18 @@
         <v>0.3</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>37126</v>
@@ -880,15 +1030,15 @@
         <v>37126</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>7</v>
@@ -906,8 +1056,520 @@
         <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>39</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0.15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>0.25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>0.7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>0.9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>0.15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>0.25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>0.25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>0.08</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>0.12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>0.08</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>0.12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>0.15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>0.25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>0.05</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>0.15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>0.6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.72</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>0.1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>157</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="4">
+        <v>157</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="4">
+        <v>9</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="4">
+        <v>90</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="4">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>15</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="4">
+        <v>40</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>0.25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="4">
+        <v>55</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>1.3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="7">
+        <v>114</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Check code validity: - check of logic in risk occurences - check logic in timber
Reorganized data:
- included data from agency
- data sorted into 3 tables:
(1) data agency: data obtained form agency (distributions; values provided in the report are given in the comment section)
(2) data etimates: data estimated/pobtained else
(3) data uncertianities: parameterized values; placeholde rvalues that are rather conceptual
</commit_message>
<xml_diff>
--- a/Data/data_agency.xlsx
+++ b/Data/data_agency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC6FF53-9794-4B01-8A11-150E8D4CC14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27A002-81DE-4999-9E22-AD8A54422E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-8460" windowWidth="14610" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="46365" yWindow="-8460" windowWidth="11340" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
   <si>
     <t>variable</t>
   </si>
@@ -113,9 +113,6 @@
     <t>fruit_price_machinery_mean_Eur</t>
   </si>
   <si>
-    <t>fruit_price_machinery_var_Eur</t>
-  </si>
-  <si>
     <t>Eur/ha</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t xml:space="preserve">Eur/tree </t>
   </si>
   <si>
-    <t>HALM 2.1 (Pflege von Agroforst, . Säule ökoregelung)</t>
-  </si>
-  <si>
     <t>HALM 2.2 (Neupflanzung/Baum, Pflanzjahr)</t>
   </si>
   <si>
@@ -158,12 +152,6 @@
     <t xml:space="preserve">NA </t>
   </si>
   <si>
-    <t>Price for walnut direct marketing (Verkaufspreis, with shell, bio)</t>
-  </si>
-  <si>
-    <t>Price for walnut wholesale market (producer price, with shell, bio)</t>
-  </si>
-  <si>
     <t>Tree planting duration in 1rst year- includes GPS, hole digging (takes longer bcs of old roots), planting (Report: 0.66 h/tree)</t>
   </si>
   <si>
@@ -200,9 +188,6 @@
     <t>Harvest machinery (shaker, collector, dryer, washer, no shell removal - Report value )</t>
   </si>
   <si>
-    <t>Variance in machinery  (20 %, own estimate)</t>
-  </si>
-  <si>
     <t>labor_fruit_pruning_juvenile_h</t>
   </si>
   <si>
@@ -263,9 +248,6 @@
     <t>Start of expading yield phase (Report: 12 Years)</t>
   </si>
   <si>
-    <t>Amount of wood to sell per tree (Report: 1.3 m^3</t>
-  </si>
-  <si>
     <t>m^3</t>
   </si>
   <si>
@@ -305,7 +287,28 @@
     <t>timber_yield_mean_m3_per_tree</t>
   </si>
   <si>
-    <t>timber_price_mean_Eur_m3</t>
+    <t>Price for walnut direct marketing (selling price == Verkaufspreis, with shell, bio)</t>
+  </si>
+  <si>
+    <t>Price for walnut wholesale market (producer price == Erzeugerpreis, with shell, bio)</t>
+  </si>
+  <si>
+    <t>Amount of wood to sell per tree (Report: 1.3 m^3)</t>
+  </si>
+  <si>
+    <t>HALM 2.1 (Pflege von Agroforst)</t>
+  </si>
+  <si>
+    <t>Variance in labor of 1rst tree planting</t>
+  </si>
+  <si>
+    <t>Labor of planting a tree in 1rst year- includes GPS, hole digging (takes longer bcs of old roots), planting (Report: 0.66 h/tree)</t>
+  </si>
+  <si>
+    <t>Discount rate over timespan of simulation</t>
+  </si>
+  <si>
+    <t>timber_price_Eur_m3</t>
   </si>
 </sst>
 </file>
@@ -363,19 +366,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -404,19 +394,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -752,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382ECF46-0337-4695-AA91-ED0309EBC33D}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,50 +768,53 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C2">
         <v>1.05</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3">
         <v>1.05</v>
       </c>
-      <c r="F2" t="s">
-        <v>37</v>
+      <c r="F2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C3">
@@ -819,21 +823,21 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4">
@@ -845,18 +849,18 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5">
@@ -865,10 +869,10 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>30</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
@@ -876,10 +880,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6">
@@ -888,21 +892,21 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>100</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>43</v>
+      <c r="G6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C7">
@@ -911,21 +915,21 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <v>0.72</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>42</v>
+      <c r="F7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8">
@@ -934,21 +938,21 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="3">
         <v>0.2</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>45</v>
+      <c r="F8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C9">
@@ -957,21 +961,21 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>1000</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>47</v>
+      <c r="G9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C10">
@@ -980,21 +984,21 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>50</v>
+      <c r="G10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C11">
@@ -1003,21 +1007,21 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>0.3</v>
       </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>51</v>
+      <c r="F11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C12">
@@ -1026,90 +1030,90 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>37126</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>54</v>
+      <c r="E13" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>0.15</v>
+        <v>0.7</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14">
-        <v>0.25</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C15">
-        <v>0.7</v>
+        <v>0.15</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
-      <c r="E15">
-        <v>0.9</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C16">
@@ -1118,44 +1122,44 @@
       <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>0.25</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="E17">
-        <v>0.25</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18">
@@ -1164,412 +1168,389 @@
       <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>0.12</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C19">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E19">
-        <v>0.12</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C20">
+        <v>0.05</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3">
         <v>0.15</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>0.25</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="F20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C21">
-        <v>0.05</v>
+        <v>0.6</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
-      <c r="E21">
-        <v>0.15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
+      <c r="E21" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>9</v>
+        <v>67</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="7">
-        <v>0.72</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>42</v>
+      <c r="E22" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3">
+        <v>157</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3">
+        <v>9</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3">
+        <v>90</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3">
+        <v>9</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27">
         <v>7</v>
       </c>
-      <c r="C23">
-        <v>0.1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24">
-        <v>157</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="4">
-        <v>157</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="4">
-        <v>9</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26">
-        <v>90</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4">
-        <v>90</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="4">
-        <v>9</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>28</v>
+      <c r="F27" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
         <v>20</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3">
+        <v>40</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>0.25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29">
+      <c r="B32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="C32">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3">
+        <v>55</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30">
-        <v>0.5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="F30" s="5" t="s">
+      <c r="G32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31">
-        <v>20</v>
-      </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="4">
-        <v>40</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="8" t="s">
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>1.3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32">
-        <v>0.25</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="8" t="s">
+      <c r="G33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C33">
-        <v>55</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="4">
-        <v>55</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="C34">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3">
+        <v>114</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" t="s">
         <v>80</v>
       </c>
-      <c r="G33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34">
-        <v>1.3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35">
-        <v>114</v>
-      </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="7">
-        <v>114</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="8"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Code: reviewed - Output plots refined - Code step-by-step reviewed again
VV function - var in %?
=> Now there's the problem that also negative values for vv series - todo: fix that!
</commit_message>
<xml_diff>
--- a/Data/data_agency.xlsx
+++ b/Data/data_agency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27A002-81DE-4999-9E22-AD8A54422E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172FA7A1-8164-46CE-BB24-305EFFBDBCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46365" yWindow="-8460" windowWidth="11340" windowHeight="15585" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
+    <workbookView xWindow="28680" yWindow="-8580" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -59,18 +59,12 @@
     <t>description</t>
   </si>
   <si>
-    <t>tnorm_0_1</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>posnorm</t>
   </si>
   <si>
-    <t>percent/100</t>
-  </si>
-  <si>
     <t>EUR/t</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>h/tree</t>
   </si>
   <si>
-    <t>Variance in 1rst tree planting</t>
-  </si>
-  <si>
     <t>tree_mainteance_costs_certificate</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
     <t>Annual costs for fertiliser per tree (Lime, compost, else; Report 6+2.2 Eur)</t>
   </si>
   <si>
-    <t>Variance in fertiliser costs</t>
-  </si>
-  <si>
     <t>tree_establishment_material_costs_per_tree</t>
   </si>
   <si>
@@ -299,9 +287,6 @@
     <t>HALM 2.1 (Pflege von Agroforst)</t>
   </si>
   <si>
-    <t>Variance in labor of 1rst tree planting</t>
-  </si>
-  <si>
     <t>Labor of planting a tree in 1rst year- includes GPS, hole digging (takes longer bcs of old roots), planting (Report: 0.66 h/tree)</t>
   </si>
   <si>
@@ -309,6 +294,21 @@
   </si>
   <si>
     <t>timber_price_Eur_m3</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>Coefficient of variation for 1rst tree planting</t>
+  </si>
+  <si>
+    <t>Coefficient of variation in fertiliser costs</t>
+  </si>
+  <si>
+    <t>Coefficient of variation for labor of 1rst tree planting</t>
   </si>
 </sst>
 </file>
@@ -411,14 +411,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -756,7 +755,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,761 +788,761 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>1.05</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3">
         <v>1.05</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>89</v>
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3">
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="3">
         <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3">
         <v>100</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>0.6</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3">
         <v>0.72</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1000</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3">
         <v>1000</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="3">
         <v>7</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="3">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>37126</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="3">
         <v>37126</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>0.15</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3">
         <v>0.25</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>0.7</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="3">
         <v>0.9</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>0.15</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="3">
         <v>0.25</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>0.15</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="3">
         <v>0.25</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>0.08</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="3">
         <v>0.12</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>0.08</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" s="3">
         <v>0.12</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>0.15</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="3">
         <v>0.25</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>0.05</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="3">
         <v>0.15</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>0.6</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="3">
         <v>0.72</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="3">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <v>157</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="3">
         <v>157</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="3">
         <v>9</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="3">
         <v>90</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="3">
         <v>9</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27">
         <v>7</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28">
         <v>15</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29">
         <v>0.5</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="3">
         <v>1.5</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="3">
         <v>40</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31">
         <v>0.25</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="3">
         <v>0.5</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32">
         <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="3">
         <v>55</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33">
         <v>1.3</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="3">
         <v>1.3</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34">
         <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" s="3">
         <v>114</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- Repository adjustments - Final model run, saved results
</commit_message>
<xml_diff>
--- a/Data/data_agency.xlsx
+++ b/Data/data_agency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heidi\ownCloud - heidi.hoffmann@stud.uni-goettingen.de@owncloud.gwdg.de\0_PA_holistic_AFP\3_code\DA_agroforestry_orchard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172FA7A1-8164-46CE-BB24-305EFFBDBCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67DE7B-A2A2-4B5E-AFFF-6AC51242699D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-8580" windowWidth="29040" windowHeight="15720" xr2:uid="{01389ECC-E809-42B1-9584-FD78A5211970}"/>
   </bookViews>
@@ -755,7 +755,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,16 +794,16 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
       </c>
       <c r="E2" s="3">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
         <v>84</v>

</xml_diff>